<commit_message>
Add New TC for Sim ATM
</commit_message>
<xml_diff>
--- a/Excel/SimATM - SCIC0009 - ATM Processing.xlsx
+++ b/Excel/SimATM - SCIC0009 - ATM Processing.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\Trial\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\1442\Desktop\ICONS\Excel\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F16BB968-22E5-4079-B8C6-02F2788DE93F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DC4AA926-6BEA-4EFA-A143-80220B81EA62}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11760" xr2:uid="{5E7B8BF1-A296-4B05-868D-4DC65ED38144}"/>
+    <workbookView xWindow="780" yWindow="780" windowWidth="15375" windowHeight="7875" xr2:uid="{5E7B8BF1-A296-4B05-868D-4DC65ED38144}"/>
   </bookViews>
   <sheets>
     <sheet name="ICON0009-001" sheetId="1" r:id="rId1"/>
@@ -472,7 +472,7 @@
   <dimension ref="A1:T4"/>
   <sheetViews>
     <sheetView showZeros="0" tabSelected="1" zoomScale="70" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="A3" sqref="A2:A3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>